<commit_message>
In vivo notebook updated
</commit_message>
<xml_diff>
--- a/data/stm_invivo/KP_5wks/KP_5wks_IDtoSampleType.xlsx
+++ b/data/stm_invivo/KP_5wks/KP_5wks_IDtoSampleType.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesse/Dropbox (MIT)/Bhatia Lab/_Projects/Lung Cancer-Share/Original Urine Data/5wks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melodi/protease_activity_analysis/data/stm_invivo/KP_5wks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8C8B38-52BA-0C48-88CA-705251847AED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19EAB57-A6F1-144E-8441-3B2092570F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1920" windowWidth="26840" windowHeight="15040" xr2:uid="{BD94B0A3-C2A4-5745-A0BF-AD20916E29CE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14240" xr2:uid="{BD94B0A3-C2A4-5745-A0BF-AD20916E29CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Control</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>C12-1A</t>
+  </si>
+  <si>
+    <t>Inj</t>
+  </si>
+  <si>
+    <t>Stock</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,7 +942,12 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>